<commit_message>
Updated index with Book2
</commit_message>
<xml_diff>
--- a/myGCFAindex.xlsx
+++ b/myGCFAindex.xlsx
@@ -3,14 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="551" documentId="11_F25DC773A252ABEACE02ECE94BDB72F45ADE5895" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{FD6F73CE-9ABA-4B1D-8EB5-6816981206A2}"/>
+  <xr:revisionPtr revIDLastSave="1168" documentId="11_F25DC773A252ABEACE02ECE94BDB72F45ADE5895" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{6387FF99-C050-438E-A726-0FCA5CB5F1F0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Book1" sheetId="1" r:id="rId1"/>
-    <sheet name="Posters" sheetId="4" r:id="rId2"/>
-    <sheet name="Volatility" sheetId="3" r:id="rId3"/>
+    <sheet name="Book2" sheetId="5" r:id="rId2"/>
+    <sheet name="Posters" sheetId="4" r:id="rId3"/>
+    <sheet name="Volatility" sheetId="3" r:id="rId4"/>
+    <sheet name="Template" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="442">
   <si>
     <t>Book</t>
   </si>
@@ -653,6 +655,1091 @@
   </si>
   <si>
     <t>Indicator of Compromise (IOC)</t>
+  </si>
+  <si>
+    <t>• Remote Access: RDP, map network shares (net.exe)
+• Remote Execution: PsExec, schtasks, services, WMI/WMIC, PSRemoting
+• Evidence of Program Execution: UserAssist, BAM/DAM, RecentApps, ShimCache, Jump Lists, Prefetch, Amcache.hve</t>
+  </si>
+  <si>
+    <t>Timestamps - Windows</t>
+  </si>
+  <si>
+    <t>• $STANDARD_INFORMATION
+• $FILENAME: all timestamps modified by file creation, file copy, volume file move (via CLI or cut/paste via Explorer)</t>
+  </si>
+  <si>
+    <t>Win For. Anal. (Red)</t>
+  </si>
+  <si>
+    <t>Open/Save MRU</t>
+  </si>
+  <si>
+    <t>• Tracks files that have been opened or saved within a Windows shell dialog box.
+• WinXP: NTUSER.DAT\Software\Microsoft\Windows\CurrentVersion\Explorer\ComDlg32\OpenSaveMRU
+• Win7/8/10: NTUSER.DAT\Software\Microsoft\Windows\CurrentVersion\Explorer\ComDlg32\OpenSavePIDIMRU</t>
+  </si>
+  <si>
+    <t>• Open/Save/MRU, Email Attachments, Skype History, Browser Artifacts, Downloads, ADS Zone.Identifier</t>
+  </si>
+  <si>
+    <t>Download of File - Artifacts</t>
+  </si>
+  <si>
+    <t>Program Execution - Artifacts</t>
+  </si>
+  <si>
+    <t>Deleted File - Artifacts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• UserAssist, Win10 Timeline, RecentApps, ShimCache, Jump Lists, Amcache.hve, BAM/DAM, Last-Visited MRU, Prefetch
+</t>
+  </si>
+  <si>
+    <t>• XP Search - ACMRU, Thumbs.db, Search - WordWheelQuery, Last-Visited MRU, Thumbcache, Recycle Bin, IE | Edge file://</t>
+  </si>
+  <si>
+    <t>Network Activity / Physical Location</t>
+  </si>
+  <si>
+    <t>File/Folder Opening</t>
+  </si>
+  <si>
+    <t>Account Usage</t>
+  </si>
+  <si>
+    <t>External Device / USB Usage</t>
+  </si>
+  <si>
+    <t>Browser Usage</t>
+  </si>
+  <si>
+    <t>Mobile For. (Blk)</t>
+  </si>
+  <si>
+    <t>SQLite</t>
+  </si>
+  <si>
+    <t>Smartphone Evidence Locations</t>
+  </si>
+  <si>
+    <t>Mobile Malware and Spyware</t>
+  </si>
+  <si>
+    <t>ADB Commands</t>
+  </si>
+  <si>
+    <t>• Requires USB debugging enabled.</t>
+  </si>
+  <si>
+    <t>libimobiledevice</t>
+  </si>
+  <si>
+    <t>• should work on locked iOS devices, but may require a trust relationship
+• ideviceinfo provides device info including encrypted state, activation status, timezone, phone number, ios version and more</t>
+  </si>
+  <si>
+    <t>Smartphone acquisition tips</t>
+  </si>
+  <si>
+    <t>• Centrally collecting and managing logs can help detect
+• Event Logs (4624 Logons, 4720 Account creation, 4776 Local account authentication, 4672 Privileged account usage), UNIX “secure” logs, auditing new accounts, anomalous logins (workstation to workstation or to/from sensitive networks), after hours logins</t>
+  </si>
+  <si>
+    <t>• Win7: UAC, Managed Service Accounts, KB2871997
+• Win8: SSP plaintext password mitigations, local admin remote logon restrictions, protected processes, restricted admin, domain protected users security group, LSA cache cleanup, group managed service accounts
+• Win10: Credential guard, remote credential guard, device guard (prevent execution of untrusted code)</t>
+  </si>
+  <si>
+    <t>Credential Guard</t>
+  </si>
+  <si>
+    <t>• Windows 10 – uses hypervisor to move domain credentials, tickets, and hashes from LSASS into isolated process</t>
+  </si>
+  <si>
+    <t>Hashes</t>
+  </si>
+  <si>
+    <t>• Password for each user account in Windows is stored in multiple formats: LM and NT most well known
+• TsPkg, Wdigest, and LiveSSP can be decrypted to provide plaintext passwords</t>
+  </si>
+  <si>
+    <t>Pass the Hash attack</t>
+  </si>
+  <si>
+    <t>• Allows an attacker to authenticate using a stolen account hash without ever knowning the clear text password
+• Several tools can facilitate: Metasploit psexec module, Windows Credential Editor (WCE), and SMBShell
+• Limited to NTLM authentication because only the hash is necessary to respond to a NTLM challenge-response protocols
+• Typically take advantage of SMB protocol to map file shares and perform PsExec remote execution</t>
+  </si>
+  <si>
+    <t>Credential Availability</t>
+  </si>
+  <si>
+    <t>Hashes - Mitigation</t>
+  </si>
+  <si>
+    <t>• Admin Action and Logon Type Code.
+• Console Logon, Runas, Remote Desktop PsExec Remote Scheduled task and Run as a Service leave credentials on target machine</t>
+  </si>
+  <si>
+    <t>• Stop remote interactive sessions with highly privileged accounts.
+• Win8: force use of restricted admin? Upgrade to Win10.
+• Win10: deploy Remote Credential Guard.</t>
+  </si>
+  <si>
+    <t>Tokens</t>
+  </si>
+  <si>
+    <t>• Every Windows process has an associated security tokens
+• Special tokens named impersonate and delegate facilitate access control and single sign on (SSO)
+• Present only when an account is logged in</t>
+  </si>
+  <si>
+    <t>Tokens – Stealing</t>
+  </si>
+  <si>
+    <t>• A user with SeImpersonate privilege (or admin/SYSTEM privileges to add it) can extract a token and reuse it to aid with things such as privilege escalation, adding users, managing group membership, mapping remote admin shares, running PsExec (delegate tokens only)
+• Common tools: incognito, Metasploit, PowerShell</t>
+  </si>
+  <si>
+    <t>Delegate Token</t>
+  </si>
+  <si>
+    <t>• Powerful authentifaction resources used for SSO, allow attackers to impersonate a user’s security context, even across network resources.</t>
+  </si>
+  <si>
+    <t>Tokens – Mitigation</t>
+  </si>
+  <si>
+    <t>• Do not interactively log into systems with highly privileged accounts
+• Accounts designated “Account is Sensitive and Cannot Be Delegated” option within AD will prevent hash storage
+• Windows 8.1+ Protected Users group do not create delegate tokens</t>
+  </si>
+  <si>
+    <t>Cached Credentials</t>
+  </si>
+  <si>
+    <t>• Common tools: Mimikatz, fgdump, gsecdump, Metasploit, SMBshell, PWDumpx, creddump, WCE (Windows Credential Editor)
+• Available in LSASS process and can be extracted with admin privileges (pre Windows 8.1)
+• Once acquired can be used in Pass the Hash attack or cracked using offline tools</t>
+  </si>
+  <si>
+    <t>Hashes – Stealing</t>
+  </si>
+  <si>
+    <t>Cached Credentials – Storage Location</t>
+  </si>
+  <si>
+    <t>• SECURITY\Cache key
+• Administrator or SYSTEM privileges required to access saved hashes, which are in mscash2 format
+• Encrypted and cannot be used in Pass the Hash attacks. Include a salt in the hash to defeat pre-computation attacks</t>
+  </si>
+  <si>
+    <t>• Stored domain credentials allow logons when the domain controller access is unavailable, by default Windows caches the last 10 logons
+• Common tools: cachedump, Metasploit, PWDumpX, creddump</t>
+  </si>
+  <si>
+    <t>Cached Credentials – Mitigation</t>
+  </si>
+  <si>
+    <t>• Reduce number of cached logon accounts in the registry key SOFTWARE\Microsoft\Windows NT\Current Version\Winlogon
+• Windows 8.1+ Domain Protected Users security group accounts do not cache credentials</t>
+  </si>
+  <si>
+    <t>Credential Attack - Mitigation</t>
+  </si>
+  <si>
+    <t>Credential Harvesting - Detection</t>
+  </si>
+  <si>
+    <t>LSA Secrets</t>
+  </si>
+  <si>
+    <t>• Credentials stored in the registry to allow services or tasks to run with user privileges
+• Commonly used to hold accounts in addition to service accounts such as RAS and VPN passwords, default login credentials, scheduled task credentials, IIS applications passwords, etc.</t>
+  </si>
+  <si>
+    <t>LSA Secrets – Stealing</t>
+  </si>
+  <si>
+    <t>LSA Secrets - Storage Location</t>
+  </si>
+  <si>
+    <t>• LSA Secrets are stored in encrypted form in the Security hive registry key SECURITY/Policy/Secrets
+• Each secret has its own key, and a parent key within SECURITY/Policy can decode the secrets.</t>
+  </si>
+  <si>
+    <t>Nishang</t>
+  </si>
+  <si>
+    <t>• The Nishang framework is designed for offensive security operations. Get-LsaSecret.ps1 can dump and decrypt LSA Secrets.</t>
+  </si>
+  <si>
+    <t>• Administrator privileges allow access to all of the encrypted registry data and the keys necessary to dump the LSA Secrets.
+• Once decrypted all passwords are in plaintext
+• Common tools: lsadump2, Cain, Metasploit, Mimikatz, gsecdump, PWDumpX, creddump</t>
+  </si>
+  <si>
+    <t>LSA Secrets – Mitigation</t>
+  </si>
+  <si>
+    <t>• Reduce number of service accounts and schedules tasks that require domain user accounts to run
+• Follow least privilege and heavily audit used accounts</t>
+  </si>
+  <si>
+    <t>Tickets</t>
+  </si>
+  <si>
+    <t>• Kerberos issues tickets to authenticated users that can be reused without additional authentication, cached in memory and valid for 10 hours</t>
+  </si>
+  <si>
+    <t>Tickets – How to Steal</t>
+  </si>
+  <si>
+    <t>• Tickets can be stolen from memory and used to impersonate users, evade the authentication process, reduce logging, authenticate elsewhere (Pass the Ticket). Common tools: Mimikatz, WCE, kerberoast
+• Access to administration account on DC can lead to creation of a ticket with no expiration (Golden Ticket)</t>
+  </si>
+  <si>
+    <t>Tickets - Attacks</t>
+  </si>
+  <si>
+    <t>Kerberos Attacks</t>
+  </si>
+  <si>
+    <t>Pass the Ticket, Overpass the hash, Kerberoasting, Golden Ticket, Silver Ticket, Skeleton key.</t>
+  </si>
+  <si>
+    <t>Pass the Ticket attack</t>
+  </si>
+  <si>
+    <t>• An attacker with administrator pivileges can dump all tickets that are cached in memory and pass them to other systems to authenticate as that acount (TGT) or service
+• Tickets can be imported into other systems allowing a user “transplant” without requiring any knowledge of hash or pwd</t>
+  </si>
+  <si>
+    <t>Golden Ticket</t>
+  </si>
+  <si>
+    <t>• Method of creating Kerberos TGT authentication ticket that does not expire
+• Can be created for any account and provides attacker with a persistent domain administrator account that would work even after full password reset of the enterprise</t>
+  </si>
+  <si>
+    <t>Tickets – Mitigation</t>
+  </si>
+  <si>
+    <t>• Hard to identify and mitigate
+• Windows 10 Credential Guard can protect by storing tickets in protected credential enclave
+• To defeat Golden Ticket attacks, krbtgt account password used by DC to create tickets must be changed twice</t>
+  </si>
+  <si>
+    <t>Pass the Ticket, Overpass the hash, Kerberoasting, Golden Ticket, Silver Ticket, Skeleton key. Mitigations on p38</t>
+  </si>
+  <si>
+    <t>NTDS.DIT</t>
+  </si>
+  <si>
+    <t>• Active Directory Domain Services database that holds all user and computer account hashes in the domain
+• “Keys to the Kingdom” that can provide access to nearly every resource in a domain
+• Located on the DC at: %SystemRoot%\NTDS folder
+• Can be extracted by loading a driver/tool to provide raw access to disk or using Volume Shadow Copy (can create if one doesnt exist) – only need administrator privileges on DC
+• SAM and SYSTEM registry hives are also necessary to facilitate decrypting the data
+• Tiiks: ntdsutil, vssadmin, ntdsxtract, metasploit, powershell, ntdsdump</t>
+  </si>
+  <si>
+    <t>NTDSXtract</t>
+  </si>
+  <si>
+    <t>• Open source tool for offline extraction of NTDS.DIT file (requires SAM and SYSTEM registry hives from DC as well)</t>
+  </si>
+  <si>
+    <t>Golden Ticket – Creation</t>
+  </si>
+  <si>
+    <t>• Administrator credentials on a domain controller is required
+• Then the has for the krbtgt account (used to create tickets) can be extracted
+• Theft of the NTDS.DIT AD database is another plausible means
+• After theft is accomplished creation of a ticket can be accomplished offline at attacker’s leisure</t>
+  </si>
+  <si>
+    <t>Prefetch</t>
+  </si>
+  <si>
+    <t>• Process in which the OS loads key pieces of data and code from disk into memory before it’s actually needed; increases system performance
+• Cache manager monitors all files and directories and maps them into a .pf file
+• Utilized to show application execution (What and When)</t>
+  </si>
+  <si>
+    <t>Prefetch – Carving</t>
+  </si>
+  <si>
+    <t>• Prefetch files are found commonly in unallocated space
+• When prefetch is collected it tends to write to new clustors instead of overwriting old
+• Therefore, can search in Unallocated for Prefetch Signature</t>
+  </si>
+  <si>
+    <t>Prefetch – Directory</t>
+  </si>
+  <si>
+    <t>• Located in C:\Windows\Prefetch
+• Populated once an application is executed, considered fairly volatile since it is updated with every program execution
+• Windows 7 and below limited to 128 files; Windows 8+ limited to 1024; Windows 10 files are compressed</t>
+  </si>
+  <si>
+    <t>Prefetch – File System Time Stamps</t>
+  </si>
+  <si>
+    <t>pecmd</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• File System timestamps of the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>“.pf”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> files can show important information:
+      • Creation date (~10 seconds) = Date/Time </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>“.exe”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> was first executed
+      • Last modification date (~10 seconds) = Date/Time </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>“.exe”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> was last executed
+• NOTE: Creation date is only best estimate, if the file was removed either by user or because of prefetch file limit then when the application runs it would create a new file, hence be inaccurate, however this rarely occurs with the 1024 limit</t>
+    </r>
+  </si>
+  <si>
+    <t>• Prefetch file analysis tool. Extracts volume info, files and directories referenced, all execution times, and total number of times the program tracked by the prefetch file was executed. Can also process an entire directory of prefetch files via the -d switch.</t>
+  </si>
+  <si>
+    <t>ShimCache</t>
+  </si>
+  <si>
+    <t>• Common term for Application Compatibility Cache (See AppCompatCache for more information).</t>
+  </si>
+  <si>
+    <t>• Designed to detect program compatility changes when a program is launched, will determine if a program needs to be “shimmed” to run application on current OS or via older OS parameters
+• Each application is checked; and will be checked again if file content is updated or renamed or moved</t>
+  </si>
+  <si>
+    <t>AppCompatCache</t>
+  </si>
+  <si>
+    <t>AppCompatCache – Location</t>
+  </si>
+  <si>
+    <t>• XP --&gt; SYSTEM\CurrentControlSet\Control\SessionManager\AppCompatibility\AppCompatCache (96 entries)
+• Server 2003/2008/20012/Win7+ --&gt; SYSTEM\CurrentControlSet\Control\SessionManager\AppCompatCache\AppCompatCache (1024 entries)</t>
+  </si>
+  <si>
+    <t>AppCompatCache – Contents</t>
+  </si>
+  <si>
+    <t>• Contains executable file’s last modification date, file path, file size
+• Windows XP tracks last execution time (last update time)
+• Vista+ contains InsertFlag that display if program was executed
+• Windows 2000 and older does not exist
+• Most recent events are on top, new entries written on shutdown</t>
+  </si>
+  <si>
+    <t>AppCompatCacheParser</t>
+  </si>
+  <si>
+    <t>• AppCompatCache execution history.
+• Used against offline SYSTEM hive or against a running system. Highest line number was executed last (lowest executed first)</t>
+  </si>
+  <si>
+    <t>AmCache.hve</t>
+  </si>
+  <si>
+    <t>• Windows 8/10 replacement of RecentFileCache.bfc</t>
+  </si>
+  <si>
+    <t>AmCache.hve – Contents</t>
+  </si>
+  <si>
+    <t>AmCache.hve – Location</t>
+  </si>
+  <si>
+    <t>• C:\Windows\AppCompat\Programs\Amcache.hve (Windows 8+, 2012+)
+• Keys = Amcache.hve\Root\File\{Volume GUID}\#####; each key represents different executable file
+• Programs installed via an installer will also have entry in: Amcache.hve\Root\Programs</t>
+  </si>
+  <si>
+    <t>• Exe full path, $Standard_Information, Last Modification Time, SHA1 hash, (sometimes – Version, ProductName, CompanyName, Description)
+• First Run Time = Last Write/Modification Time of key
+• SHA-1 hash of executable also contained in the key.</t>
+  </si>
+  <si>
+    <t>AmcacheParser</t>
+  </si>
+  <si>
+    <t>• Extracts Amcache information: first run time of executable, SHA-1, full path of executable</t>
+  </si>
+  <si>
+    <t>Event Logs – Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Original .evt logs: %SystemRoot%\System32\config
+• Revamped .evtx logs: %SystemRoot%\System32\winevt\logs; can also be sent to a remote log collector
+• Admin can designate locations for individual logs with certain registry keys. </t>
+  </si>
+  <si>
+    <t>Event Logs – Types</t>
+  </si>
+  <si>
+    <t>• 3 primary logs (originally began with only these): Security Logs, System Logs, Application Logs
+• 1 “Custom” category that includes additional logs such as Directory Service, File Replication, DNS Server</t>
+  </si>
+  <si>
+    <t>Event Logs – Types – System</t>
+  </si>
+  <si>
+    <t>• Contains events related to Windows services, system components, drivers, resources, etc
+• Example: Service stopped, system rebooted</t>
+  </si>
+  <si>
+    <t>• Custom application logs
+• Examples: Server logs such as Directory Services, DNS Server, File Replication Service</t>
+  </si>
+  <si>
+    <t>Event Logs - Types - Custom</t>
+  </si>
+  <si>
+    <t>Event Logs - Types - Application</t>
+  </si>
+  <si>
+    <t>• Software events unrelated to OS.
+• Example: SQL server fails to access a database.</t>
+  </si>
+  <si>
+    <t>Event Logs - Types - Security</t>
+  </si>
+  <si>
+    <t>Event Logs - Types - Applications and Services</t>
+  </si>
+  <si>
+    <t>• Comprises of all the new “custom” logs that are application specific
+• Things such as – Remote Desktop logs, Windows Firewall logs, Windows Defender logs, PowerShell logs, etc…
+• Logs often go further back in time than System, Security, and Application logs</t>
+  </si>
+  <si>
+    <t>• Only updated by the LSASS process
+• Only user accounts with administrator permissions can review, export, or clear
+• Most useful log in forensics – contains user authentication and logon, behavior and actions, file/folder/share access, security settings modifications, and can log both success and failure if selected</t>
+  </si>
+  <si>
+    <t>• Security logs include the following categories: Account logon, Account management, Directory service access, Logon events, Object access, Policy change, Privilege user, Process Tracking, System events</t>
+  </si>
+  <si>
+    <t>Event Logs - Types - Security Event Categories</t>
+  </si>
+  <si>
+    <t>Account Usage - Tracking</t>
+  </si>
+  <si>
+    <t>• Used to determine which accounts have been used for attempted logons. Track account usage for known compromised accounts
+• See Event ID Chart: Related Security Log ID’s = 4624, 4625, 4634, 4647, 4648, 4672, 4720
+• Windows XP Event ID’s = 528-552</t>
+  </si>
+  <si>
+    <t>eventvwr.exe</t>
+  </si>
+  <si>
+    <t>• Windows Event Viewer</t>
+  </si>
+  <si>
+    <t>Logon Type Codes</t>
+  </si>
+  <si>
+    <t>• Most common types 2 (console), 3 (network), 10 (RDP). For others see chart.</t>
+  </si>
+  <si>
+    <t>• Each account session is assigned a unique Logon ID at time of logon and can be used for tracking session length (logon to logoff comparison) and user activities during the session
+• Useful Event ID’s: 4624 (logon), 4647 (logoff), 4634 (logoff) and corresponding XP ID’s: 528, 538, 551</t>
+  </si>
+  <si>
+    <t>Logon Sessions - Tracking</t>
+  </si>
+  <si>
+    <t>Built-In Accounts</t>
+  </si>
+  <si>
+    <t>• Windows has built-in service accounts that are used to allow processes to run within different security contexts.
+• Many processes run without user interaction or before user even logs on
+• System, Local Service, Network Service, &lt;hostname&gt;$, DWM, UMFD, Anonymous Logon</t>
+  </si>
+  <si>
+    <t>Privileged/Admin Activity</t>
+  </si>
+  <si>
+    <t>• Accounts assigned privileges associated with an administrator will trigger a 4672 event to be logged
+     • Does not have to be full admin, can include privileges like SeTakeOwnership, SeDebug, and SeImpersonate
+• Event ID 4624 (successful logon) followed by the 4672 can be attributed to an admin account logging into system. (WinXP event ID: 576)</t>
+  </si>
+  <si>
+    <t>Account Creation</t>
+  </si>
+  <si>
+    <t>• Event ID 4720 recorded for account creation. Contains: Date, time, computer created on, account that authorized creation, and account details
+• Same event is used for both local and domain account creation
+• See Event ID Chart for complimentary events: 4722, 4724, 4728, 4732, 4735, 4738, 4756 (WinXP event: 624)</t>
+  </si>
+  <si>
+    <t>RDP</t>
+  </si>
+  <si>
+    <t>• 4778 and 4779 track RDP session connection/disconnection. Records IP address and hostname of the system that established the session
+• Will also contain logon/logoff events as credentials are passed/accepted by system
+• 4778/4779 is also used in Windows “Fast User Switching” feature but seassion name will be “Console”
+• RDP application specific logs (RDPCoreTS ID 131 and TerminalServices-RemoteControlManager ID 1149) can be used
+• Windows XP: 682, 683</t>
+  </si>
+  <si>
+    <t>RDP - Logging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• RDP activity is logged in multiple places - Security log, and some custom logs. Understanding source/destination is critical. </t>
+  </si>
+  <si>
+    <t>Account Logon</t>
+  </si>
+  <si>
+    <t>• Different from Logon Events, which are stored locally on the actual system being logged into.
+• Account Logon Events are stored on system who authorized logon (DC for domain, local system for non-domain)
+• Includes logging on and logging off</t>
+  </si>
+  <si>
+    <t>Account Logon Events</t>
+  </si>
+  <si>
+    <t>• Refer to third-party authorization of credentials provided during the logon session, username/password must be vailidated by the domain controller using either NTLM or Kerberos authentication protocols
+• NTLM Event ID codes: 4776 (successful/failed authentication
+• Kerberos Event ID codes: 4768 (TGT – successful logon); 4769 (ST requested – acess to srvr resource); 4771 (failed logon)
+• Windows XP Event ID’s: 672, 673, 675, 680</t>
+  </si>
+  <si>
+    <t>Account Logon Error Codes</t>
+  </si>
+  <si>
+    <t>• Event ID 4771 signifies failed Kerberos authentication.(WinXP: 675). 40+ error codes can be issued.
+• Event ID 4776 signifies failed NTLM authentication (WinXP: 680,529). Contains error code generated and stored in the Event Description.
+• See Logon Error Codes chart.</t>
+  </si>
+  <si>
+    <t>Enumeration - Account and Group</t>
+  </si>
+  <si>
+    <t>• 4798: user's local group membership was enumerated.
+• 4799: security-enabled local group membership was enumerated.</t>
+  </si>
+  <si>
+    <t>Event Log Explorer</t>
+  </si>
+  <si>
+    <t>• Third-part event log management software package that supports .evt and .evtx formats allowing it to be a useful GUI log parser
+• Very capable of working with corrupted logs, has robust filtering capability, allows many log files to be opened simultaneously and even merged aiding with event correlation, and color coding by Event ID’s</t>
+  </si>
+  <si>
+    <t>Network Shares</t>
+  </si>
+  <si>
+    <t>• Event logs can be used to audit activity around network shares
+• Must be enabled: “Object Access --&gt; Audit File Share” option within Advanced Audit Policy Configuration
+          • Event ID 5140 associated with this auditing and will records any access to network shares on the system
+                    • Includes: Share name, logon account, remote IP address
+          • Event ID’s 5142-5144 tracks shares that have been created, modified, or deleted
+• To log file access on a network share “Object Access --&gt; Audit Detailed File Share” must be enabled
+          • Event ID’s 5145 will record individual item acces – VERY noisy and only recommended for very sensitive systems</t>
+  </si>
+  <si>
+    <t>Scheduled Tasks logs</t>
+  </si>
+  <si>
+    <t>• Identify and audit scheduled tasks; includes events from both the Microsoft-Windows-Task Scheduler/Operational (TskSch) log and Security (Sec) log…...Format for Event ID’s below: “Description” (TskSch | Sec)
+• Scheduled Task Created (106 | 4698);     Scheduled Task Updated (140 | 4702);     Scheduled Task Deleted (141 | 4699) Scheduled Task Executed/Completed ( 200 &amp; 201 | $null); Scheduled task enabled/disabled ($null | 4700 &amp; 4701). Windows XP: 602</t>
+  </si>
+  <si>
+    <t>TaskScheduler Log</t>
+  </si>
+  <si>
+    <t>• Can help serve as an additional location to track user account logons, because entries persist longer than in Security log. 
+• Important event IDs: 106 (newly created schtasks), 200/201 (task executed/completed)</t>
+  </si>
+  <si>
+    <t>Task Scheduler v1.0</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">• Original scheduled task format, found in XP/Win2003 systems and older
+• Stores </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.job</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> files (in binary format) in the %SystemRoot%\Tasks folder
+• Contains: Registration date/time, user account, full command path, execution date/time</t>
+    </r>
+  </si>
+  <si>
+    <t>at.exe</t>
+  </si>
+  <si>
+    <t>• Used to locally or remotely schedule tasks
+• Leaves behind .job files which indicate what was scheduled and who scheduled it; Also Event Log evidence</t>
+  </si>
+  <si>
+    <t>• New scheduled task format implemented in Vista+ and Server 2008+
+• File with same name as task is created in %SystemRoot%\system32\Tasks folder with no extension in XML format
+• Contains: Account used to register task, and account authenticated to run task. 
+• RegistrationInfo (Author tag) can identify remote system name and account used to register task (only for remote)</t>
+  </si>
+  <si>
+    <t>Task Scheduler v1.2 artifacts</t>
+  </si>
+  <si>
+    <t>• Analyze logs for suspicious services running at boot time, or review services started/stopped during time of suspected hack
+• System Logs: 7034 (service crashed), 7035 (service sent start/stop control), 7036 (service started/stopped), 7040 (start type changed), 7045 (service installed on system)
+• Security log: 4697 (service installed on system)
+          • NOTE: “Audit Security System Extension” must be selected via local or group policy for Security Event ID’s to exist
+• Windows XP: 7034, 7035, 7036, 7040</t>
+  </si>
+  <si>
+    <t>Services - Suspicious Services</t>
+  </si>
+  <si>
+    <t>Event Log Clearing</t>
+  </si>
+  <si>
+    <t>• Easy to determine whether even logs have been modified
+• Local administrators, domain administrators, and SYSTEM account have privileges to clear event logs
+• Individual records can not be selectively removed – the entire log must be removed
+• Event ID 1102 (Security Log) is triggered when Security Log is cleared and ID 104 is triggered in the System Log when any other log is cleared</t>
+  </si>
+  <si>
+    <t>Event Log Attacks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Selective deletion possible with DanderSpritz eventlogedit or Mimikatz evvent::drop, but preliminary. </t>
+  </si>
+  <si>
+    <t>• RDP is the most common remote desktop protocol in Windows networks. Also look for VNC, TeamViewer.
+• Check …RDPClient/Operational log, presence of the file Default.rdp in a user's profile</t>
+  </si>
+  <si>
+    <t>• Best logs are located on destination machine: Event logs (4624 logon type 10 (RDP); logon type 2 (VNC), 4778/4779 RDP session events), Process tracking (Event ID 4688, RDPClip.exe)</t>
+  </si>
+  <si>
+    <t>• Default shared resources designed to allow administrative programs access to the entire file system
+• Present on every modern version of Windows (hidden) and almost always enabled
+• Common shares: DriveLetter$ (C$, D$, etc.), Admin$ IPC$</t>
+  </si>
+  <si>
+    <t>Admin Shares</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">• Event logs: 4624 Logon type 3, 4672 privilege account usage, 5140 network share accessed
+• Command line auditing (for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>net use</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> or similar commands), Network forensics
+• Registry: NTUSER\Software\Microsoft\Windows\CurrentVersion\Explorer\MountPoints2 (on source system)</t>
+    </r>
+  </si>
+  <si>
+    <t>C$</t>
+  </si>
+  <si>
+    <t>Drive volume share</t>
+  </si>
+  <si>
+    <t>Admin$</t>
+  </si>
+  <si>
+    <t>• Hidden admin share that gives complete access to the Windows folder</t>
+  </si>
+  <si>
+    <t>IPC$</t>
+  </si>
+  <si>
+    <t>• Hidden admin share used by named pipes</t>
+  </si>
+  <si>
+    <t>Admin Shares - Destination Artifacts</t>
+  </si>
+  <si>
+    <t>Admin Shares – Source Artifacts</t>
+  </si>
+  <si>
+    <t>• Domain administrator privileges or the built-in admin account (RID 500) are required for remote access to admin shares
+• Search for event ID 4624 type 3 (network logons) and corresponding 5140 share access events.</t>
+  </si>
+  <si>
+    <t>PsExec</t>
+  </si>
+  <si>
+    <t>• Designed by Microsoft SysInternals to be a lightweight tool for remote administration operations
+• Can push and execute code non-interactively, make built-in system commands “remote-capable”, used for interactive console sessions
+• Can authenticate to target system, mount hidden ADMIN$ share, copy PsExeSvc.exe and any other binaries necessary to Windows folder, starts PSEXESVC and executes commands, named pipes are used to communicate b/w target and source
+• Leaves significant forensic artifacts</t>
+  </si>
+  <si>
+    <t>• NTUSER\Software\SysInternals\PsExec\EulaAccepted registry key. 
+• Event ID 4648 "runas" event created on source system. Full command line if command line auditing is enabled.
+• Running processes and memory analysis (PSExec.exe)
+• Prefetch, BAM/DAM, AmCache.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• 4624 Type 3 or Type 2 (network vs console with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>“-u”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> option)
+• 5140 due to PsExec mounting ADMIN$ share
+• Creation, Starting, Stopping of PSEXESVC service also writes several events to the System log
+• Creation of PsExec service creates key: SYSTEM\CurrentControlSet\Services\PSEXESVC</t>
+    </r>
+  </si>
+  <si>
+    <t>• PSEXEC.EXE (source) and PSEXESVC.EXE (target) processes in memory
+• PsExec also establishes three name pipes to facilitate communication that can be retrieved via handles in memory:
+          • \\&lt;source ip&gt;\pipe\PSEXESVC-&lt;hostname&gt;-&lt;PID&gt;-stdin (one also for stdout and stderr same syntax)</t>
+  </si>
+  <si>
+    <t>PsExec – Destination Memory Artifacts</t>
+  </si>
+  <si>
+    <t>Remote Management Tools</t>
+  </si>
+  <si>
+    <t>• Windows includes several tools capable of remote execution – sc.exe, schtasks.exe, at.exe, reg.exe, winrs.exe</t>
+  </si>
+  <si>
+    <t>sc.exe</t>
+  </si>
+  <si>
+    <t>• Used to create, start, stop, manage local or remote services
+• Activity is recorded in registry and include the binary that was executed; Also stored in event log</t>
+  </si>
+  <si>
+    <t>schtasks.exe</t>
+  </si>
+  <si>
+    <t>• Used to locally or remotely schedule tasks
+• Leaves behind evidence of what was scheduled and who scheduled it; Also Event Log evidence</t>
+  </si>
+  <si>
+    <t>reg.exe</t>
+  </si>
+  <si>
+    <t>• Used to interact with local or remote registry
+• Remote Registry service must be started on target and prior authentication accomplished (i.e., mount an admin share)
+• Registry key last write times can help detection</t>
+  </si>
+  <si>
+    <t>winrs.exe</t>
+  </si>
+  <si>
+    <t>• If Windows Remote Management (WinRM) service is enabled it can run any arbitrary command with defaul encrypted traffic
+• Will often be able to pass through firewalls where PsExec might otherwise fail
+• Detection can be the WinRM service started if that is against the normal for environment OR winrshost.exe process on remote system</t>
+  </si>
+  <si>
+    <t>• Most common WMI command for lateral movement is “process call create”
+• Leaves behind fewer artifacts with similar capabilities to PsExec
+• WMI traffic is typically not encrypted so network forensics can be useful for tracking usage</t>
+  </si>
+  <si>
+    <t>WMI - Source Artifacts</t>
+  </si>
+  <si>
+    <t>PSExec - Destination  Artifacts</t>
+  </si>
+  <si>
+    <t>PsExec - Source  Artifacts</t>
+  </si>
+  <si>
+    <t>RDP - Source  Artifacts</t>
+  </si>
+  <si>
+    <t>RDP - Destination  Artifacts</t>
+  </si>
+  <si>
+    <t>WMI - Destination Artifacts</t>
+  </si>
+  <si>
+    <t>• Application execution artifacts (Prefetch and Shimcache) on the target machine – wmiprvse.exe
+• Event logs – EID 4624 Type 3 (network logon) events
+• New Microsoft-Windows-WMI-Activity/Operational log provides evidence of remote WMI activity.
+• Residue from WMI event consumers: creation of MOF files or execution of mofcomp.exe</t>
+  </si>
+  <si>
+    <t>PowerShell Remoting - Source Artifacts</t>
+  </si>
+  <si>
+    <t>• Most common PowerShell commands for lateral movement: Invoke-Command and Enter-PSSession (latter provides encrypted interactive shell similar to SSH)
+• Microsoft-Windows-PowerShell/Operational log can identify PS sessions. Microsoft-Windows-WinRM/Operational can identify remote PS activity.
+• PowerShell console history log ConsoleHost_history.txt records last 4096 commands typed per user on soruce system.</t>
+  </si>
+  <si>
+    <t>PowerShell Remoting - Destination Artifacts</t>
+  </si>
+  <si>
+    <t>• Application execution artifacts (Prefetch/Shimcache) on target machine – wmiprvse.exe, powershell.exe, wsmprovhost.exe
+• Event logs – EID 4624 Type 3 (network logon) events
+• Process tracking and command line auditing
+• PowerShell v5 contains detailed script block logging and logging suspicious activity by default</t>
+  </si>
+  <si>
+    <t>Application Deployment Software</t>
+  </si>
+  <si>
+    <t>• Most enterprise environments have implemented automated patching utilities.
+• Possibility for attackers to gain access to the deployment server, create deployment package, and distribute it across the network.
+• Similar type of attack can be conducted through cloud control panels which provide full control of entire cloud infrastructure.</t>
+  </si>
+  <si>
+    <t>Vulnerability Exploitation</t>
+  </si>
+  <si>
+    <t>• Exploiting vulnerabilities to provide shell access or allow remove code execution, can also include post-exploitation malware installation
+• Account logon auditing is ineffective
+• Common examples: Poison Ivy, PlugX, Gh0stRat, webshells, Metasploit Meterpreter</t>
+  </si>
+  <si>
+    <t>Malware Execution</t>
+  </si>
+  <si>
+    <t>• Identify potential malware and determine if it was executed
+• Security log can log event ID’s 4688 (executed process) and 4689 (process termination) if auditing is enabled
+          • Rarely enabled due to large amount of noise (except critical systems)
+• System and Application logs – Windows Error Reporting events can identify troubled applications and even blue screen
+          • Application Event ID 1000 (application errors) and 1002 (application hangs), also look for Error and Warning events
+          • System log Event ID 1001 – Windows Error Reporting events
+• Windows XP: 592 (Security log)</t>
+  </si>
+  <si>
+    <t>Process Tracking</t>
+  </si>
+  <si>
+    <t>• Detailed tracking information for events. Relevant event IDs: 4688 (new process created, incl. executable path), 4689 (process exit)
+• Examples: program activation, process exit, handle duplications, indirect object access, etc…</t>
+  </si>
+  <si>
+    <t>Command line</t>
+  </si>
+  <si>
+    <t>• Microsoft introducted a group policy setting to enable recording of full command lines in process reporting (Server 2012R2 and later backported to Windows 7+)
+• Requires successful process creation auditing to be enabled
+• 4688 – Process creation event</t>
+  </si>
+  <si>
+    <t>• PowerShell v5 introduced script block logging capability. Can capture full command or script contents, who executed it, when it was executed
+• Enabled via Administrative Template (Group Policy) – NOT enabled by default
+• Microsoft-Windows-PowerShell/Operational log: 4103 (module logging &amp; pipeline output), 4104 (script contents) 4105/4106 (script start/stop)
+• NOTE: PowerShell has built-in feature that will automatically log suspicious scripts (even if script block logging is disabled)</t>
+  </si>
+  <si>
+    <t>CyberChef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Web app for encryption, encoding and compression analysis. Excellent for identifying and decoding a wide range of obfuscation. </t>
+  </si>
+  <si>
+    <t>PowerShell - Script Block Logging</t>
+  </si>
+  <si>
+    <t>PowerShell - Transcript Logs</t>
+  </si>
+  <si>
+    <t>• Logs all commands typed and output. Only records input/output to the PowerShell terminal. Different from Script Block logging.
+• Written to Users\&lt;account&gt;\Documents by default</t>
+  </si>
+  <si>
+    <t>PSReadline</t>
+  </si>
+  <si>
+    <t>ConsoleHost_history.txt</t>
+  </si>
+  <si>
+    <t>• Where PSReadline commands are stored.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Default module designed to log last 4096 commands typed into PowerShell console. Commands stored in user's profile ConsoleHost_history.txt
+• Attackers can disable or remove PSReadline module. </t>
+  </si>
+  <si>
+    <t>WMI Persistence - Auditing</t>
+  </si>
+  <si>
+    <t>• Easily audit for malicious WMI event consumer persistence, by reviewing the WMI-Activity/Operational log.
+• Event ID 5857-5861 record filter/consumer activity. 5861 is most useful - new permanent event consumer creation.</t>
+  </si>
+  <si>
+    <t>• Chart. Event logs and IDs corresponding to logons, account logon, RDP, network shares, scheduled tasks, installation, services, log clearing, malware execution, command lines, WMI</t>
+  </si>
+  <si>
+    <t>Event Logs - Extraction</t>
+  </si>
+  <si>
+    <t>Event Logs - Log + ID Summary</t>
+  </si>
+  <si>
+    <t>• Event logs can be exported either from a live system or offline
+• Live system methods: Export from event viewer and save file (.evt, .evtx, .csv, .xml, .txt formats), remote extraction using SIFT Workstation and FTK imager (can result in corrupted logs) or using SysInternals PsLogList tool (commandline tool for dumping live logs in text or .csv file)
+• Offline system methods: Event Log Explorer (Windows), evtwalk or evtx_parser (SIFT), EVTXtract carving tool</t>
+  </si>
+  <si>
+    <t>Event Viewer</t>
+  </si>
+  <si>
+    <t>• Event viewer can be used to export event logs from a live system. Can be saved in .evt, .evtx, .csv, .xml, .txt formats</t>
+  </si>
+  <si>
+    <t>PsLogList</t>
+  </si>
+  <si>
+    <t>• SysInternal command-line tool used to dump live logs to a text or csv file, read and output exported event logs in their native .evt/.evtx format, pre-filter output, dump event logs from remote systems
+• Live system extraction/export</t>
+  </si>
+  <si>
+    <t>evtwalk</t>
+  </si>
+  <si>
+    <t>• Offline log parser that can read binary logs from Event Viewer and output text</t>
+  </si>
+  <si>
+    <t>evtx</t>
+  </si>
+  <si>
+    <t>evtx_parser</t>
+  </si>
+  <si>
+    <t>evtx_view</t>
+  </si>
+  <si>
+    <t>EVTXtract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Dedicated event log carver focused on EVTX records. Can work with offline logs. </t>
+  </si>
+  <si>
+    <t>Get-WinEvent</t>
+  </si>
+  <si>
+    <t>PowerShell - Get Event Logs</t>
+  </si>
+  <si>
+    <t>• PowerShell gives native access to event logs. Get-WinEvent should be used with the modern EVTX format. Can collect from remote systems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• PowerShell gives native access to event logs. Get-WinEvent should be used with the modern EVTX format. Can collect from remote systems.
+• Get-EventLog was previously used for older "classic" logs. </t>
+  </si>
+  <si>
+    <t>Event Logs - Scaling Collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Microsoft Windows Event Forwarding is a free capability to collect and centralize logs.
+• Winlogbeat: open-source forwarding solution designed to work with ElasticSearch. Splunk Universal Forwarder: commercial solution. </t>
+  </si>
+  <si>
+    <t>Sysmon</t>
+  </si>
+  <si>
+    <t>• Free logging extension from Microsoft. Easy installation and configuration. Result is new event log Microsoft-Windows-Sysmon/Operational</t>
   </si>
 </sst>
 </file>
@@ -685,7 +1772,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -746,6 +1833,24 @@
         <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF92D050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFCC99FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -774,7 +1879,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -833,6 +1938,28 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1116,8 +2243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2398,16 +3525,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F11418F-1EAA-4E38-9942-4E8AF066F20F}">
-  <dimension ref="A1:D23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F9AC0C8-0260-4037-B50A-70D5588A8C36}">
+  <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="100.140625" customWidth="1"/>
@@ -2427,143 +3554,1739 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="7"/>
+    <row r="2" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7">
+        <v>6</v>
+      </c>
       <c r="C2" s="8" t="s">
-        <v>92</v>
+        <v>234</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>8</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24">
+        <v>2</v>
+      </c>
+      <c r="B4" s="25">
+        <v>9</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7">
+        <v>10</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>2</v>
+      </c>
+      <c r="B6" s="7">
+        <v>10</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7">
+        <v>10</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7">
+        <v>12</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>2</v>
+      </c>
+      <c r="B9" s="6">
+        <v>17</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>2</v>
+      </c>
+      <c r="B10" s="7">
+        <v>19</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>2</v>
+      </c>
+      <c r="B11" s="7">
+        <v>19</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>2</v>
+      </c>
+      <c r="B12" s="7">
+        <v>19</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>2</v>
+      </c>
+      <c r="B13" s="7">
+        <v>22</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>2</v>
+      </c>
+      <c r="B14" s="7">
+        <v>24</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>2</v>
+      </c>
+      <c r="B15" s="7">
+        <v>24</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>2</v>
+      </c>
+      <c r="B16" s="7">
+        <v>27</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>2</v>
+      </c>
+      <c r="B17" s="7">
+        <v>28</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>2</v>
+      </c>
+      <c r="B18" s="7">
+        <v>28</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>2</v>
+      </c>
+      <c r="B19" s="7">
+        <v>28</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>2</v>
+      </c>
+      <c r="B20" s="6">
+        <v>29</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>2</v>
+      </c>
+      <c r="B21" s="7">
+        <v>30</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>2</v>
+      </c>
+      <c r="B22" s="7">
+        <v>31</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>2</v>
+      </c>
+      <c r="B23" s="7">
+        <v>31</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>2</v>
+      </c>
+      <c r="B24" s="6">
+        <v>34</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>2</v>
+      </c>
+      <c r="B25" s="6">
+        <v>34</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>2</v>
+      </c>
+      <c r="B26" s="7">
+        <v>34</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>2</v>
+      </c>
+      <c r="B27" s="7">
+        <v>34</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
+        <v>2</v>
+      </c>
+      <c r="B28" s="7">
+        <v>35</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
+        <v>2</v>
+      </c>
+      <c r="B29" s="7">
+        <v>36</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>2</v>
+      </c>
+      <c r="B30" s="7">
+        <v>39</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
+        <v>2</v>
+      </c>
+      <c r="B31" s="7">
+        <v>39</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
+        <v>2</v>
+      </c>
+      <c r="B32" s="20">
+        <v>42</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
+        <v>2</v>
+      </c>
+      <c r="B33" s="20">
+        <v>42</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
+        <v>2</v>
+      </c>
+      <c r="B34" s="20">
+        <v>42</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="9">
+        <v>2</v>
+      </c>
+      <c r="B35" s="20">
+        <v>45</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>2</v>
+      </c>
+      <c r="B36" s="6">
+        <v>47</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="9">
+        <v>2</v>
+      </c>
+      <c r="B37" s="20">
+        <v>51</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="9">
+        <v>2</v>
+      </c>
+      <c r="B38" s="20">
+        <v>51</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="9">
+        <v>2</v>
+      </c>
+      <c r="B39" s="20">
+        <v>51</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="9">
+        <v>2</v>
+      </c>
+      <c r="B40" s="20">
+        <v>51</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="9">
+        <v>2</v>
+      </c>
+      <c r="B41" s="9">
+        <v>54</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="17">
+        <v>2</v>
+      </c>
+      <c r="B42" s="17">
+        <v>55</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>285</v>
+      </c>
+      <c r="D42" s="28" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="17">
+        <v>2</v>
+      </c>
+      <c r="B43" s="17">
+        <v>55</v>
+      </c>
+      <c r="C43" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="D43" s="28" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="17">
+        <v>2</v>
+      </c>
+      <c r="B44" s="17">
+        <v>55</v>
+      </c>
+      <c r="C44" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="D44" s="28" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>2</v>
+      </c>
+      <c r="B45" s="9">
+        <v>58</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="9">
+        <v>2</v>
+      </c>
+      <c r="B46" s="9">
+        <v>64</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="9">
+        <v>2</v>
+      </c>
+      <c r="B47" s="9">
+        <v>66</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="9">
+        <v>2</v>
+      </c>
+      <c r="B48" s="9">
+        <v>66</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="9">
+        <v>2</v>
+      </c>
+      <c r="B49" s="9">
+        <v>66</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="15">
+        <v>2</v>
+      </c>
+      <c r="B50" s="16">
+        <v>66</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="15">
+        <v>2</v>
+      </c>
+      <c r="B51" s="16">
+        <v>67</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="17">
+        <v>2</v>
+      </c>
+      <c r="B52" s="18">
+        <v>68</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="9">
+        <v>2</v>
+      </c>
+      <c r="B53" s="9">
+        <v>69</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="9">
+        <v>2</v>
+      </c>
+      <c r="B54" s="9">
+        <v>73</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="9">
+        <v>2</v>
+      </c>
+      <c r="B55" s="9">
+        <v>74</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="9">
+        <v>2</v>
+      </c>
+      <c r="B56" s="9">
+        <v>77</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="9">
+        <v>2</v>
+      </c>
+      <c r="B57" s="9">
+        <v>79</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>2</v>
+      </c>
+      <c r="B58" s="4">
+        <v>83</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="9">
+        <v>2</v>
+      </c>
+      <c r="B59" s="9">
+        <v>85</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="9">
+        <v>2</v>
+      </c>
+      <c r="B60" s="9">
+        <v>87</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>2</v>
+      </c>
+      <c r="B61" s="4">
+        <v>89</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>2</v>
+      </c>
+      <c r="B62" s="4">
         <v>93</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="C62" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="9">
+        <v>2</v>
+      </c>
+      <c r="B63" s="9">
+        <v>95</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A64" s="9">
+        <v>2</v>
+      </c>
+      <c r="B64" s="9">
+        <v>95</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="9">
+        <v>2</v>
+      </c>
+      <c r="B65" s="9">
+        <v>96</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
+        <v>2</v>
+      </c>
+      <c r="B66" s="4">
+        <v>100</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="9">
+        <v>2</v>
+      </c>
+      <c r="B67" s="9">
+        <v>103</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="9">
+        <v>2</v>
+      </c>
+      <c r="B68" s="9">
+        <v>106</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A69" s="9">
+        <v>2</v>
+      </c>
+      <c r="B69" s="9">
+        <v>112</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
+        <v>2</v>
+      </c>
+      <c r="B70" s="4">
+        <v>114</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="9">
+        <v>2</v>
+      </c>
+      <c r="B71" s="7">
+        <v>114</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="9">
+        <v>2</v>
+      </c>
+      <c r="B72" s="7">
+        <v>114</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" s="9">
+        <v>2</v>
+      </c>
+      <c r="B73" s="7">
+        <v>117</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A74" s="9">
+        <v>2</v>
+      </c>
+      <c r="B74" s="9">
+        <v>119</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A75" s="9">
+        <v>2</v>
+      </c>
+      <c r="B75" s="9">
+        <v>123</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
+        <v>2</v>
+      </c>
+      <c r="B76" s="4">
+        <v>126</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A77" s="9">
+        <v>2</v>
+      </c>
+      <c r="B77" s="7">
+        <v>130</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A78" s="3">
+        <v>2</v>
+      </c>
+      <c r="B78" s="4">
+        <v>132</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="3">
+        <v>2</v>
+      </c>
+      <c r="B79" s="18">
+        <v>133</v>
+      </c>
+      <c r="C79" s="19" t="s">
+        <v>358</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="9">
+        <v>2</v>
+      </c>
+      <c r="B80" s="7">
+        <v>133</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="3">
+        <v>2</v>
+      </c>
+      <c r="B81" s="4">
+        <v>133</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="3">
+        <v>2</v>
+      </c>
+      <c r="B82" s="4">
+        <v>133</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="3">
+        <v>2</v>
+      </c>
+      <c r="B83" s="4">
+        <v>133</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="3">
+        <v>2</v>
+      </c>
+      <c r="B84" s="4">
+        <v>134</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A85" s="9">
+        <v>2</v>
+      </c>
+      <c r="B85" s="7">
+        <v>136</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A86" s="3">
+        <v>2</v>
+      </c>
+      <c r="B86" s="4">
+        <v>136</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A87" s="3">
+        <v>2</v>
+      </c>
+      <c r="B87" s="4">
+        <v>137</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="9">
+        <v>2</v>
+      </c>
+      <c r="B88" s="7">
+        <v>138</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A89" s="9">
+        <v>2</v>
+      </c>
+      <c r="B89" s="7">
+        <v>139</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A90" s="9">
+        <v>2</v>
+      </c>
+      <c r="B90" s="7">
+        <v>141</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A91" s="9">
+        <v>2</v>
+      </c>
+      <c r="B91" s="7">
+        <v>142</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="D91" s="8" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A92" s="9">
+        <v>2</v>
+      </c>
+      <c r="B92" s="7">
+        <v>140</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A93" s="9">
+        <v>2</v>
+      </c>
+      <c r="B93" s="7">
+        <v>140</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="D93" s="8" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A94" s="9">
+        <v>2</v>
+      </c>
+      <c r="B94" s="7">
+        <v>143</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A95" s="9">
+        <v>2</v>
+      </c>
+      <c r="B95" s="7">
+        <v>144</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A96" s="9">
+        <v>2</v>
+      </c>
+      <c r="B96" s="7">
+        <v>145</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A97" s="9">
+        <v>2</v>
+      </c>
+      <c r="B97" s="7">
+        <v>147</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="9">
+        <v>2</v>
+      </c>
+      <c r="B98" s="7">
+        <v>148</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A99" s="9">
+        <v>2</v>
+      </c>
+      <c r="B99" s="7">
+        <v>150</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A100" s="9">
+        <v>2</v>
+      </c>
+      <c r="B100" s="9">
+        <v>155</v>
+      </c>
+      <c r="C100" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A101" s="9">
+        <v>2</v>
+      </c>
+      <c r="B101" s="9">
+        <v>158</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A102" s="9">
+        <v>2</v>
+      </c>
+      <c r="B102" s="9">
+        <v>158</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A103" s="9">
+        <v>2</v>
+      </c>
+      <c r="B103" s="9">
+        <v>164</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="D103" s="8" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="9">
+        <v>2</v>
+      </c>
+      <c r="B104" s="7">
+        <v>171</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A105" s="9">
+        <v>2</v>
+      </c>
+      <c r="B105" s="7">
+        <v>173</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A106" s="9">
+        <v>2</v>
+      </c>
+      <c r="B106" s="7">
+        <v>176</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A107" s="9">
+        <v>2</v>
+      </c>
+      <c r="B107" s="7">
+        <v>176</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="D107" s="8" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A108" s="9">
+        <v>2</v>
+      </c>
+      <c r="B108" s="7">
+        <v>177</v>
+      </c>
+      <c r="C108" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D108" s="8" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A109" s="9">
+        <v>2</v>
+      </c>
+      <c r="B109" s="7">
+        <v>182</v>
+      </c>
+      <c r="C109" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A110" s="9">
+        <v>2</v>
+      </c>
+      <c r="B110" s="7">
+        <v>183</v>
+      </c>
+      <c r="C110" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="D110" s="8" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="9">
+        <v>2</v>
+      </c>
+      <c r="B111" s="9">
+        <v>183</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>423</v>
+      </c>
+      <c r="D111" s="8" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A112" s="9">
+        <v>2</v>
+      </c>
+      <c r="B112" s="9">
+        <v>183</v>
+      </c>
+      <c r="C112" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="D112" s="8" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="9">
+        <v>2</v>
+      </c>
+      <c r="B113" s="9">
+        <v>183</v>
+      </c>
+      <c r="C113" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="D113" s="8" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="9">
+        <v>2</v>
+      </c>
+      <c r="B114" s="9">
+        <v>183</v>
+      </c>
+      <c r="C114" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="D114" s="8" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="9">
+        <v>2</v>
+      </c>
+      <c r="B115" s="9">
+        <v>183</v>
+      </c>
+      <c r="C115" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="9">
+        <v>2</v>
+      </c>
+      <c r="B116" s="9">
+        <v>183</v>
+      </c>
+      <c r="C116" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="D116" s="8" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="9">
+        <v>2</v>
+      </c>
+      <c r="B117" s="7">
+        <v>184</v>
+      </c>
+      <c r="C117" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="D117" s="8" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A118" s="9">
+        <v>2</v>
+      </c>
+      <c r="B118" s="7">
+        <v>185</v>
+      </c>
+      <c r="C118" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="D118" s="8" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A119" s="9">
+        <v>2</v>
+      </c>
+      <c r="B119" s="7">
+        <v>185</v>
+      </c>
+      <c r="C119" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="D119" s="8" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A120" s="9">
+        <v>2</v>
+      </c>
+      <c r="B120" s="7">
+        <v>186</v>
+      </c>
+      <c r="C120" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="D120" s="8" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A121" s="9">
+        <v>2</v>
+      </c>
+      <c r="B121" s="7">
+        <v>188</v>
+      </c>
+      <c r="C121" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="D121" s="8" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="9"/>
+      <c r="B122" s="7"/>
+      <c r="C122" s="8"/>
+      <c r="D122" s="8"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="9"/>
+      <c r="B123" s="7"/>
+      <c r="C123" s="8"/>
+      <c r="D123" s="8"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="9"/>
+      <c r="B124" s="7"/>
+      <c r="C124" s="8"/>
+      <c r="D124" s="8"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="9"/>
+      <c r="B125" s="7"/>
+      <c r="C125" s="8"/>
+      <c r="D125" s="8"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="9"/>
+      <c r="B126" s="7"/>
+      <c r="C126" s="8"/>
+      <c r="D126" s="8"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="9"/>
+      <c r="B127" s="7"/>
+      <c r="C127" s="8"/>
+      <c r="D127" s="8"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="9"/>
+      <c r="B128" s="7"/>
+      <c r="C128" s="8"/>
+      <c r="D128" s="8"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="9"/>
+      <c r="B129" s="7"/>
+      <c r="C129" s="8"/>
+      <c r="D129" s="8"/>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="3"/>
+      <c r="B130" s="4"/>
+      <c r="C130" s="5"/>
+      <c r="D130" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2572,6 +5295,264 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F11418F-1EAA-4E38-9942-4E8AF066F20F}">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" style="23" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="100.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="22"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="22"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="71" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD08527-4024-49B1-AFDC-8CDEB4761439}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2583,4 +5564,574 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6D0CAA-7282-4901-B278-1ADA98A21B6C}">
+  <dimension ref="A1:D90"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="100.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="15"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="17"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="17"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="17"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="15"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="5"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="15"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="15"/>
+      <c r="B72" s="20"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="15"/>
+      <c r="B73" s="20"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="3"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="3"/>
+      <c r="B78" s="18"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="19"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="3"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="3"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="3"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="3"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="3"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="3"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="3"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="3"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="3"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="3"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="3"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="3"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="71" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>